<commit_message>
reshaped repo and added plots
</commit_message>
<xml_diff>
--- a/data/TDP_Dataset.xlsx
+++ b/data/TDP_Dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\Desktop\TDP_project\TDP-phylogenetic-analysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\OneDrive - Politecnico di Milano\TDP_project\rev0\TDP-phylogenetic-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5504989A-02EA-4C2B-B86A-220E2E07C9E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A35F9D-46C8-4643-9DD2-6AD8DB2E5E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22440" yWindow="1665" windowWidth="15375" windowHeight="7875" firstSheet="3" activeTab="4" xr2:uid="{E069122C-ED96-4935-AB31-689319DFB304}"/>
+    <workbookView xWindow="-27630" yWindow="-1440" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{E069122C-ED96-4935-AB31-689319DFB304}"/>
   </bookViews>
   <sheets>
     <sheet name="TDP1alpha Dataset" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
     <sheet name="Classification beta-bt" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Classification alpha -bt'!$A$1:$D$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Classification alpha -bt'!$A$1:$D$175</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Classification alpha -NJ'!$A$1:$D$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Classification beta'!$A$1:$D$37</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TDP1alpha Dataset'!$A$2:$F$158</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'TDP1beta dataset'!$A$2:$F$59</definedName>
   </definedNames>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="549">
   <si>
     <t>Class</t>
   </si>
@@ -1762,6 +1763,9 @@
   </si>
   <si>
     <t>Ancestral plants, gymno</t>
+  </si>
+  <si>
+    <t>Classification</t>
   </si>
 </sst>
 </file>
@@ -6063,9 +6067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A05531-38C3-4427-9AD7-B44C5545A8F2}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
@@ -6090,7 +6095,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
@@ -6104,7 +6109,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>400</v>
       </c>
@@ -6118,7 +6123,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>401</v>
       </c>
@@ -6132,7 +6137,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>402</v>
       </c>
@@ -6146,7 +6151,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>403</v>
       </c>
@@ -6160,7 +6165,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>404</v>
       </c>
@@ -6174,7 +6179,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>405</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>406</v>
       </c>
@@ -6202,7 +6207,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>407</v>
       </c>
@@ -6216,7 +6221,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>408</v>
       </c>
@@ -6230,7 +6235,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>409</v>
       </c>
@@ -6244,7 +6249,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>410</v>
       </c>
@@ -6258,7 +6263,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>411</v>
       </c>
@@ -6272,7 +6277,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>412</v>
       </c>
@@ -6286,7 +6291,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>413</v>
       </c>
@@ -6300,7 +6305,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>414</v>
       </c>
@@ -6314,7 +6319,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>415</v>
       </c>
@@ -6328,7 +6333,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
         <v>416</v>
       </c>
@@ -6342,7 +6347,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
         <v>417</v>
       </c>
@@ -6356,7 +6361,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>418</v>
       </c>
@@ -6370,7 +6375,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>419</v>
       </c>
@@ -6384,7 +6389,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>420</v>
       </c>
@@ -6398,7 +6403,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>498</v>
       </c>
@@ -6412,7 +6417,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>421</v>
       </c>
@@ -6426,7 +6431,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>422</v>
       </c>
@@ -6440,7 +6445,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>423</v>
       </c>
@@ -6454,7 +6459,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>424</v>
       </c>
@@ -6468,7 +6473,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
         <v>425</v>
       </c>
@@ -6482,7 +6487,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>426</v>
       </c>
@@ -6496,7 +6501,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>427</v>
       </c>
@@ -6510,7 +6515,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>428</v>
       </c>
@@ -6524,7 +6529,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>429</v>
       </c>
@@ -6538,7 +6543,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>430</v>
       </c>
@@ -6552,7 +6557,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>431</v>
       </c>
@@ -6566,7 +6571,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>500</v>
       </c>
@@ -6580,7 +6585,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>432</v>
       </c>
@@ -6594,7 +6599,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>433</v>
       </c>
@@ -6608,7 +6613,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
         <v>434</v>
       </c>
@@ -6622,7 +6627,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
         <v>435</v>
       </c>
@@ -6636,7 +6641,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>436</v>
       </c>
@@ -6650,7 +6655,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
         <v>437</v>
       </c>
@@ -6664,7 +6669,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
         <v>438</v>
       </c>
@@ -6678,7 +6683,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
         <v>439</v>
       </c>
@@ -6692,7 +6697,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
         <v>440</v>
       </c>
@@ -6706,7 +6711,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
         <v>441</v>
       </c>
@@ -6720,7 +6725,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
         <v>442</v>
       </c>
@@ -6734,7 +6739,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
         <v>443</v>
       </c>
@@ -6748,7 +6753,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
         <v>444</v>
       </c>
@@ -6860,7 +6865,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="41" t="s">
         <v>452</v>
       </c>
@@ -6874,7 +6879,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="38" t="s">
         <v>453</v>
       </c>
@@ -6888,7 +6893,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="s">
         <v>456</v>
       </c>
@@ -6902,7 +6907,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="41" t="s">
         <v>457</v>
       </c>
@@ -6916,7 +6921,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="40" t="s">
         <v>458</v>
       </c>
@@ -6930,7 +6935,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="41" t="s">
         <v>459</v>
       </c>
@@ -6944,7 +6949,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
         <v>460</v>
       </c>
@@ -6958,7 +6963,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="s">
         <v>461</v>
       </c>
@@ -6972,7 +6977,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="s">
         <v>499</v>
       </c>
@@ -6986,7 +6991,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
         <v>462</v>
       </c>
@@ -7000,7 +7005,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="41" t="s">
         <v>463</v>
       </c>
@@ -7014,7 +7019,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="s">
         <v>470</v>
       </c>
@@ -7028,7 +7033,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="40" t="s">
         <v>464</v>
       </c>
@@ -7042,7 +7047,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="40" t="s">
         <v>465</v>
       </c>
@@ -7056,7 +7061,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="40" t="s">
         <v>466</v>
       </c>
@@ -7070,7 +7075,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="41" t="s">
         <v>467</v>
       </c>
@@ -7084,7 +7089,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="41" t="s">
         <v>469</v>
       </c>
@@ -7098,7 +7103,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="40" t="s">
         <v>468</v>
       </c>
@@ -7112,7 +7117,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
         <v>454</v>
       </c>
@@ -7126,7 +7131,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="s">
         <v>455</v>
       </c>
@@ -7140,7 +7145,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="s">
         <v>520</v>
       </c>
@@ -7154,7 +7159,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
         <v>522</v>
       </c>
@@ -7168,7 +7173,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
         <v>484</v>
       </c>
@@ -7182,7 +7187,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="40" t="s">
         <v>485</v>
       </c>
@@ -7196,7 +7201,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="41" t="s">
         <v>486</v>
       </c>
@@ -7210,7 +7215,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="s">
         <v>487</v>
       </c>
@@ -7224,7 +7229,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
         <v>523</v>
       </c>
@@ -7238,7 +7243,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="s">
         <v>493</v>
       </c>
@@ -7252,7 +7257,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="41" t="s">
         <v>494</v>
       </c>
@@ -7266,7 +7271,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="s">
         <v>495</v>
       </c>
@@ -7280,7 +7285,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
         <v>496</v>
       </c>
@@ -7294,7 +7299,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="s">
         <v>501</v>
       </c>
@@ -7308,7 +7313,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="41" t="s">
         <v>497</v>
       </c>
@@ -7323,7 +7328,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D89" xr:uid="{E1BAB694-70B3-4415-A39E-85435B6AAC8C}"/>
+  <autoFilter ref="A1:D89" xr:uid="{E1BAB694-70B3-4415-A39E-85435B6AAC8C}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Eudicots, Brassicales"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -7331,17 +7342,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22626E32-7929-439D-A6BD-5A1BCC7554F9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="39.85546875" customWidth="1"/>
-    <col min="3" max="4" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -7358,7 +7371,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>484</v>
       </c>
@@ -7372,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>545</v>
       </c>
@@ -7386,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>485</v>
       </c>
@@ -7400,7 +7413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>487</v>
       </c>
@@ -7414,7 +7427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="s">
         <v>468</v>
       </c>
@@ -7428,7 +7441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>455</v>
       </c>
@@ -7442,7 +7455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
         <v>522</v>
       </c>
@@ -7456,7 +7469,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>454</v>
       </c>
@@ -7470,7 +7483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>520</v>
       </c>
@@ -7484,7 +7497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>497</v>
       </c>
@@ -7498,7 +7511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>495</v>
       </c>
@@ -7512,7 +7525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>496</v>
       </c>
@@ -7526,7 +7539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>493</v>
       </c>
@@ -7540,7 +7553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>494</v>
       </c>
@@ -7554,7 +7567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>501</v>
       </c>
@@ -8366,7 +8379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="40" t="s">
         <v>523</v>
       </c>
@@ -8380,7 +8393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
         <v>469</v>
       </c>
@@ -8394,7 +8407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="41" t="s">
         <v>466</v>
       </c>
@@ -8405,10 +8418,10 @@
         <v>22</v>
       </c>
       <c r="D76" s="41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="s">
         <v>467</v>
       </c>
@@ -8419,10 +8432,10 @@
         <v>22</v>
       </c>
       <c r="D77" s="41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
         <v>464</v>
       </c>
@@ -8433,10 +8446,10 @@
         <v>22</v>
       </c>
       <c r="D78" s="41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="41" t="s">
         <v>465</v>
       </c>
@@ -8447,10 +8460,10 @@
         <v>22</v>
       </c>
       <c r="D79" s="41">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="40" t="s">
         <v>456</v>
       </c>
@@ -8464,7 +8477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="41" t="s">
         <v>543</v>
       </c>
@@ -8478,7 +8491,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="41" t="s">
         <v>462</v>
       </c>
@@ -8492,7 +8505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
         <v>470</v>
       </c>
@@ -8506,7 +8519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="s">
         <v>544</v>
       </c>
@@ -8520,7 +8533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="41" t="s">
         <v>457</v>
       </c>
@@ -8534,7 +8547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="s">
         <v>460</v>
       </c>
@@ -8548,7 +8561,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
         <v>458</v>
       </c>
@@ -8562,7 +8575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="41" t="s">
         <v>459</v>
       </c>
@@ -8576,7 +8589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="41" t="s">
         <v>461</v>
       </c>
@@ -8590,7 +8603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="66" t="s">
         <v>546</v>
       </c>
@@ -8604,7 +8617,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="66" t="s">
         <v>546</v>
       </c>
@@ -8618,7 +8631,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="66" t="s">
         <v>546</v>
       </c>
@@ -8632,7 +8645,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="66" t="s">
         <v>546</v>
       </c>
@@ -8646,7 +8659,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="66" t="s">
         <v>546</v>
       </c>
@@ -8660,7 +8673,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="66" t="s">
         <v>546</v>
       </c>
@@ -8674,7 +8687,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="66" t="s">
         <v>546</v>
       </c>
@@ -8688,7 +8701,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="66" t="s">
         <v>546</v>
       </c>
@@ -8702,7 +8715,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="66" t="s">
         <v>546</v>
       </c>
@@ -8716,7 +8729,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="66" t="s">
         <v>546</v>
       </c>
@@ -8730,7 +8743,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="66" t="s">
         <v>546</v>
       </c>
@@ -8744,7 +8757,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="66" t="s">
         <v>546</v>
       </c>
@@ -8758,7 +8771,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="66" t="s">
         <v>546</v>
       </c>
@@ -8772,7 +8785,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="66" t="s">
         <v>546</v>
       </c>
@@ -8786,7 +8799,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="66" t="s">
         <v>546</v>
       </c>
@@ -8800,7 +8813,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="66" t="s">
         <v>546</v>
       </c>
@@ -8814,7 +8827,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="66" t="s">
         <v>546</v>
       </c>
@@ -8828,7 +8841,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="66" t="s">
         <v>546</v>
       </c>
@@ -8842,7 +8855,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="66" t="s">
         <v>546</v>
       </c>
@@ -8856,7 +8869,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="66" t="s">
         <v>546</v>
       </c>
@@ -8870,7 +8883,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="66" t="s">
         <v>546</v>
       </c>
@@ -8884,7 +8897,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="66" t="s">
         <v>546</v>
       </c>
@@ -8898,7 +8911,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="66" t="s">
         <v>546</v>
       </c>
@@ -8912,7 +8925,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="66" t="s">
         <v>546</v>
       </c>
@@ -8926,7 +8939,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="66" t="s">
         <v>546</v>
       </c>
@@ -8940,7 +8953,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="66" t="s">
         <v>546</v>
       </c>
@@ -8954,7 +8967,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="66" t="s">
         <v>546</v>
       </c>
@@ -8968,7 +8981,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="66" t="s">
         <v>546</v>
       </c>
@@ -8982,7 +8995,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="66" t="s">
         <v>546</v>
       </c>
@@ -8996,7 +9009,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="66" t="s">
         <v>546</v>
       </c>
@@ -9010,7 +9023,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="66" t="s">
         <v>546</v>
       </c>
@@ -9024,7 +9037,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="66" t="s">
         <v>546</v>
       </c>
@@ -9038,7 +9051,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="66" t="s">
         <v>546</v>
       </c>
@@ -9052,7 +9065,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="66" t="s">
         <v>546</v>
       </c>
@@ -9066,7 +9079,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="66" t="s">
         <v>546</v>
       </c>
@@ -9080,7 +9093,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="66" t="s">
         <v>546</v>
       </c>
@@ -9094,7 +9107,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="66" t="s">
         <v>546</v>
       </c>
@@ -9108,7 +9121,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="66" t="s">
         <v>546</v>
       </c>
@@ -9122,7 +9135,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="66" t="s">
         <v>546</v>
       </c>
@@ -9136,7 +9149,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="66" t="s">
         <v>546</v>
       </c>
@@ -9150,7 +9163,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="66" t="s">
         <v>546</v>
       </c>
@@ -9164,7 +9177,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="66" t="s">
         <v>546</v>
       </c>
@@ -9178,7 +9191,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="66" t="s">
         <v>546</v>
       </c>
@@ -9192,7 +9205,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="66" t="s">
         <v>546</v>
       </c>
@@ -9206,7 +9219,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="66" t="s">
         <v>546</v>
       </c>
@@ -9220,7 +9233,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="66" t="s">
         <v>546</v>
       </c>
@@ -9234,7 +9247,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="66" t="s">
         <v>546</v>
       </c>
@@ -9248,7 +9261,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="66" t="s">
         <v>546</v>
       </c>
@@ -9262,7 +9275,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="66" t="s">
         <v>546</v>
       </c>
@@ -9276,7 +9289,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="66" t="s">
         <v>546</v>
       </c>
@@ -9290,7 +9303,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="66" t="s">
         <v>546</v>
       </c>
@@ -9304,7 +9317,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="66" t="s">
         <v>546</v>
       </c>
@@ -9318,7 +9331,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="66" t="s">
         <v>546</v>
       </c>
@@ -9332,7 +9345,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="66" t="s">
         <v>546</v>
       </c>
@@ -9346,7 +9359,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="66" t="s">
         <v>546</v>
       </c>
@@ -9360,7 +9373,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="66" t="s">
         <v>546</v>
       </c>
@@ -9374,7 +9387,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="66" t="s">
         <v>546</v>
       </c>
@@ -9388,7 +9401,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="66" t="s">
         <v>546</v>
       </c>
@@ -9402,7 +9415,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="66" t="s">
         <v>546</v>
       </c>
@@ -9416,7 +9429,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="66" t="s">
         <v>546</v>
       </c>
@@ -9430,7 +9443,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="66" t="s">
         <v>546</v>
       </c>
@@ -9444,7 +9457,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="66" t="s">
         <v>546</v>
       </c>
@@ -9458,7 +9471,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="66" t="s">
         <v>546</v>
       </c>
@@ -9472,7 +9485,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="66" t="s">
         <v>546</v>
       </c>
@@ -9486,7 +9499,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="66" t="s">
         <v>546</v>
       </c>
@@ -9500,7 +9513,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="66" t="s">
         <v>546</v>
       </c>
@@ -9514,7 +9527,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="66" t="s">
         <v>546</v>
       </c>
@@ -9528,7 +9541,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="66" t="s">
         <v>546</v>
       </c>
@@ -9542,7 +9555,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="66" t="s">
         <v>546</v>
       </c>
@@ -9556,7 +9569,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="66" t="s">
         <v>546</v>
       </c>
@@ -9570,7 +9583,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="66" t="s">
         <v>546</v>
       </c>
@@ -9584,7 +9597,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="66" t="s">
         <v>546</v>
       </c>
@@ -9598,7 +9611,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="66" t="s">
         <v>546</v>
       </c>
@@ -9612,7 +9625,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="66" t="s">
         <v>546</v>
       </c>
@@ -9626,7 +9639,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="66" t="s">
         <v>546</v>
       </c>
@@ -9640,7 +9653,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="66" t="s">
         <v>546</v>
       </c>
@@ -9654,7 +9667,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="66" t="s">
         <v>546</v>
       </c>
@@ -9668,7 +9681,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="66" t="s">
         <v>546</v>
       </c>
@@ -9682,7 +9695,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="66" t="s">
         <v>546</v>
       </c>
@@ -9696,7 +9709,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="66" t="s">
         <v>546</v>
       </c>
@@ -9710,7 +9723,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="66" t="s">
         <v>546</v>
       </c>
@@ -9724,7 +9737,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="66" t="s">
         <v>546</v>
       </c>
@@ -9738,7 +9751,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="66" t="s">
         <v>546</v>
       </c>
@@ -9752,7 +9765,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="66" t="s">
         <v>546</v>
       </c>
@@ -9766,7 +9779,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="66" t="s">
         <v>546</v>
       </c>
@@ -9780,7 +9793,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="66" t="s">
         <v>546</v>
       </c>
@@ -9795,7 +9808,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D89" xr:uid="{E1BAB694-70B3-4415-A39E-85435B6AAC8C}">
+  <autoFilter ref="A1:D175" xr:uid="{E1BAB694-70B3-4415-A39E-85435B6AAC8C}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Eudicots, Asterids"/>
+        <filter val="Eudicots, Caryophyllales"/>
+        <filter val="Eudicots, Ranunculales"/>
+        <filter val="Eudicots, Rosids"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D89">
       <sortCondition ref="B2:B89"/>
     </sortState>
@@ -10900,10 +10921,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDFD3B6-C6C3-4FD6-B7A4-DC69E550924D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11026,7 +11048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
         <v>427</v>
       </c>
@@ -11040,7 +11062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>422</v>
       </c>
@@ -11054,7 +11076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>430</v>
       </c>
@@ -11068,7 +11090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
         <v>418</v>
       </c>
@@ -11082,7 +11104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>489</v>
       </c>
@@ -11096,7 +11118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>417</v>
       </c>
@@ -11110,7 +11132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41" t="s">
         <v>420</v>
       </c>
@@ -11124,7 +11146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
         <v>498</v>
       </c>
@@ -11138,7 +11160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41" t="s">
         <v>412</v>
       </c>
@@ -11152,7 +11174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
         <v>411</v>
       </c>
@@ -11166,7 +11188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
         <v>440</v>
       </c>
@@ -11180,7 +11202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
         <v>448</v>
       </c>
@@ -11194,7 +11216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
         <v>445</v>
       </c>
@@ -11208,7 +11230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
         <v>449</v>
       </c>
@@ -11222,7 +11244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>450</v>
       </c>
@@ -11236,7 +11258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
         <v>431</v>
       </c>
@@ -11250,7 +11272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>409</v>
       </c>
@@ -11264,7 +11286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
         <v>453</v>
       </c>
@@ -11278,7 +11300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
         <v>425</v>
       </c>
@@ -11292,7 +11314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>438</v>
       </c>
@@ -11306,7 +11328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>437</v>
       </c>
@@ -11320,7 +11342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>460</v>
       </c>
@@ -11334,7 +11356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>461</v>
       </c>
@@ -11348,7 +11370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>458</v>
       </c>
@@ -11362,7 +11384,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41" t="s">
         <v>457</v>
       </c>
@@ -11376,7 +11398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>463</v>
       </c>
@@ -11390,7 +11412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>462</v>
       </c>
@@ -11404,7 +11426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
         <v>454</v>
       </c>
@@ -11418,7 +11440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>468</v>
       </c>
@@ -11433,6 +11455,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D37" xr:uid="{CDD3AA02-D210-47E7-8275-E62A4343214B}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Eudicots, Fabales"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -11442,8 +11471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3750FC99-DF1D-443C-AD78-42D0E0431DA4}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11452,6 +11481,7 @@
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -11459,7 +11489,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>377</v>
+        <v>548</v>
       </c>
       <c r="C1" s="31" t="s">
         <v>502</v>
@@ -11974,6 +12004,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>